<commit_message>
tests: updated test data 2
</commit_message>
<xml_diff>
--- a/tests/data/pump_example_with_missing_cells_raise_issues.xlsx
+++ b/tests/data/pump_example_with_missing_cells_raise_issues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{807EB21E-6D4E-4A4C-BD87-FC837AC5811A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A41F1D-ACE9-4ADD-BE0F-A64ECBBBD146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="198">
   <si>
     <t>role</t>
   </si>
@@ -102,15 +102,9 @@
     <t>Value Type</t>
   </si>
   <si>
-    <t>Nullable</t>
-  </si>
-  <si>
     <t>Immutable</t>
   </si>
   <si>
-    <t>Is List</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -616,6 +610,15 @@
   </si>
   <si>
     <t>Pu mp</t>
+  </si>
+  <si>
+    <t>Max Count</t>
+  </si>
+  <si>
+    <t>Min Count</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -1019,13 +1022,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1065,12 +1068,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>45638.469729340279</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>45638.469729340279</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1118,24 +1121,24 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="41.5" customWidth="1"/>
-    <col min="5" max="5" width="30.5" customWidth="1"/>
-    <col min="6" max="6" width="37.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.44140625" customWidth="1"/>
+    <col min="6" max="6" width="37.44140625" customWidth="1"/>
     <col min="7" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="26.5" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" customWidth="1"/>
     <col min="13" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1155,7 +1158,7 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1175,39 +1178,39 @@
         <v>24</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
@@ -1218,20 +1221,20 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="6" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
       </c>
       <c r="H3" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="b">
-        <v>0</v>
+      <c r="I3" s="6">
+        <v>1</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
@@ -1240,114 +1243,114 @@
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="6" t="b">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
       </c>
       <c r="H4" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="6" t="b">
-        <v>1</v>
+      <c r="I4" s="6">
+        <v>100</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="6" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
       </c>
       <c r="H5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="6" t="b">
-        <v>0</v>
+      <c r="I5" s="6">
+        <v>1</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="7" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
       </c>
       <c r="H6" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="7" t="b">
-        <v>0</v>
+      <c r="I6" s="7">
+        <v>1</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>10</v>
@@ -1356,30 +1359,32 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="7" t="b">
-        <v>1</v>
+      <c r="I7" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1388,12 +1393,12 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
@@ -1404,20 +1409,20 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="7" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
       </c>
       <c r="H8" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="7" t="b">
-        <v>0</v>
+      <c r="I8" s="7">
+        <v>1</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
@@ -1426,68 +1431,70 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="7" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
       </c>
       <c r="H9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="7" t="b">
-        <v>0</v>
+      <c r="I9" s="7">
+        <v>1</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="6" t="b">
-        <v>1</v>
+      <c r="I10" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -1496,10 +1503,10 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1516,10 +1523,10 @@
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1535,53 +1542,53 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="6" t="b">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
       </c>
       <c r="H13" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="6" t="b">
-        <v>0</v>
+      <c r="I13" s="6">
+        <v>1</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>8</v>
@@ -1592,20 +1599,20 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="6" t="b">
-        <v>1</v>
+        <v>34</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
       </c>
       <c r="H14" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="6" t="b">
-        <v>0</v>
+      <c r="I14" s="6">
+        <v>1</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>8</v>
@@ -1614,170 +1621,170 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="6" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
       </c>
       <c r="H15" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="6" t="b">
-        <v>0</v>
+      <c r="I15" s="6">
+        <v>1</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="6" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
       </c>
       <c r="H16" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="6" t="b">
-        <v>0</v>
+      <c r="I16" s="6">
+        <v>1</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="6" t="b">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
       </c>
       <c r="H17" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="6" t="b">
-        <v>0</v>
+      <c r="I17" s="6">
+        <v>1</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="6" t="b">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
       </c>
       <c r="H18" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="6" t="b">
-        <v>0</v>
+      <c r="I18" s="6">
+        <v>1</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="P19" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1794,18 +1801,18 @@
       <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.5" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="4" width="70" customWidth="1"/>
     <col min="5" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1815,7 +1822,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -1826,587 +1833,587 @@
         <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
         <v>82</v>
       </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
         <v>84</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="D6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
         <v>88</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>89</v>
       </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="D7" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>91</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>92</v>
       </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="C8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8" t="s">
         <v>94</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
         <v>95</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>96</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="C9" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
         <v>98</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>99</v>
       </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>100</v>
       </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="C10" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
         <v>102</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>103</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>104</v>
       </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="C11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
         <v>106</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>107</v>
       </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="C12" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
         <v>109</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>110</v>
       </c>
-      <c r="D12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="C13" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
         <v>112</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>113</v>
       </c>
-      <c r="F13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="C14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
         <v>115</v>
       </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>116</v>
       </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="B15" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>118</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>120</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>121</v>
       </c>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="C16" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
         <v>123</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>124</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
         <v>125</v>
       </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="C17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>127</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
         <v>128</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>129</v>
       </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="B18" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
         <v>131</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
         <v>132</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>133</v>
       </c>
-      <c r="D18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="B19" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
         <v>135</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
         <v>136</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>137</v>
       </c>
-      <c r="D19" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="C20" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
         <v>139</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>140</v>
       </c>
-      <c r="D20" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="C21" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
         <v>142</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>143</v>
       </c>
-      <c r="D21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="D22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>145</v>
       </c>
-      <c r="D22" t="s">
-        <v>112</v>
-      </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="C23" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
         <v>147</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
         <v>148</v>
       </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>150</v>
       </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="B25" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
         <v>152</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
         <v>153</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>154</v>
       </c>
-      <c r="D25" t="s">
-        <v>125</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="B27" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
         <v>156</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
         <v>157</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
         <v>158</v>
       </c>
-      <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="F27" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="C28" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
         <v>160</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>161</v>
       </c>
-      <c r="D28" t="s">
-        <v>125</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="B29" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
         <v>163</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
         <v>164</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>165</v>
       </c>
-      <c r="D29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="C30" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="D30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
         <v>167</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>168</v>
       </c>
-      <c r="D30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="C31" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
         <v>170</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>171</v>
       </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="C32" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
         <v>173</v>
       </c>
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>174</v>
       </c>
-      <c r="D32" t="s">
-        <v>104</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
         <v>176</v>
       </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="C34" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
+        <v>123</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
         <v>178</v>
       </c>
-      <c r="C34" t="s">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>179</v>
       </c>
-      <c r="D34" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="C35" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
         <v>181</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>182</v>
       </c>
-      <c r="D35" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="C36" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
         <v>184</v>
       </c>
-      <c r="C36" t="s">
-        <v>185</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H37" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2423,17 +2430,17 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2441,9 +2448,9 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
@@ -2452,46 +2459,46 @@
         <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2508,28 +2515,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>21</v>
@@ -2538,7 +2545,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2555,28 +2562,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>21</v>
@@ -2585,7 +2592,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>